<commit_message>
update Report 3 + sửa lại tên DDL_Checklist_Test Case Review_v1.0_EN.xlsx
</commit_message>
<xml_diff>
--- a/WIP/Documents/Report 3/DDL_Checklist_Test Case Review_v1.0_EN.xlsx
+++ b/WIP/Documents/Report 3/DDL_Checklist_Test Case Review_v1.0_EN.xlsx
@@ -196,19 +196,19 @@
     <t>[   X  ] - Pass</t>
   </si>
   <si>
-    <t>Project Code: FAP</t>
-  </si>
-  <si>
-    <t>Reviewer(s):ThuyLM</t>
-  </si>
-  <si>
-    <t>Review date: :&lt;19-07-2015&gt;</t>
-  </si>
-  <si>
     <t>Effort spent on review (man-hour):3</t>
   </si>
   <si>
     <t>Work product' size:</t>
+  </si>
+  <si>
+    <t>Reviewer(s):ChinhVC</t>
+  </si>
+  <si>
+    <t>Review date: :&lt;20-11-2015&gt;</t>
+  </si>
+  <si>
+    <t>Project Code: DDL</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>

</xml_diff>